<commit_message>
updated Business Startup Cost
</commit_message>
<xml_diff>
--- a/Documentation/Business Startup Cost .xlsx
+++ b/Documentation/Business Startup Cost .xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jana Marie Gardon\Documents\College\4thyr-1st term\Tentrep\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlbel\Desktop\Project---TENTREP\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8508" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="pre" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="64">
   <si>
     <t>Pre-operational Expenses</t>
   </si>
@@ -217,15 +217,18 @@
   <si>
     <t>Tourist Arrival in the Philippines</t>
   </si>
+  <si>
+    <t>18-month extension Operational Cost</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_([$PHP]\ * #,##0_);_([$PHP]\ * \(#,##0\);_([$PHP]\ * &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_([$PHP]\ * #,##0.00_);_([$PHP]\ * \(#,##0.00\);_([$PHP]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_([$PHP]\ * #,##0_);_([$PHP]\ * \(#,##0\);_([$PHP]\ * &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_([$PHP]\ * #,##0.00_);_([$PHP]\ * \(#,##0.00\);_([$PHP]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -378,14 +381,14 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -394,18 +397,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -427,26 +430,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="4"/>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="3" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="3" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="1" xfId="5" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="6" applyBorder="1" applyAlignment="1">
@@ -454,6 +457,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -775,28 +781,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
@@ -810,7 +816,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -825,7 +831,7 @@
         <v>36000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>52</v>
       </c>
@@ -840,7 +846,7 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -855,7 +861,7 @@
         <v>2413</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
@@ -870,7 +876,7 @@
         <v>7188.2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
@@ -885,7 +891,7 @@
         <v>10272.84</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
@@ -900,7 +906,7 @@
         <v>8740</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
@@ -915,7 +921,7 @@
         <v>3920</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="5"/>
       <c r="D10" s="3"/>
@@ -924,13 +930,13 @@
         <v>188534.04</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -947,7 +953,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>16</v>
       </c>
@@ -961,7 +967,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>17</v>
       </c>
@@ -975,7 +981,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>18</v>
       </c>
@@ -989,7 +995,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
       <c r="D16" s="3"/>
@@ -997,184 +1003,163 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B18" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C18" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D18" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G18" s="14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="11" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C19" s="17">
         <v>30000</v>
-      </c>
-      <c r="D18" s="3">
-        <v>4</v>
-      </c>
-      <c r="E18" s="17">
-        <f>C18*D18</f>
-        <v>120000</v>
-      </c>
-      <c r="G18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="17">
-        <v>26666</v>
       </c>
       <c r="D19" s="3">
         <v>4</v>
       </c>
       <c r="E19" s="17">
         <f>C19*D19</f>
-        <v>106664</v>
+        <v>120000</v>
       </c>
       <c r="G19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="11" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C20" s="17">
-        <v>16000</v>
+        <v>26666</v>
       </c>
       <c r="D20" s="3">
         <v>4</v>
       </c>
       <c r="E20" s="17">
         <f>C20*D20</f>
-        <v>64000</v>
+        <v>106664</v>
       </c>
       <c r="G20" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="11" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="C21" s="17">
-        <v>21500</v>
+        <v>16000</v>
       </c>
       <c r="D21" s="3">
         <v>4</v>
       </c>
       <c r="E21" s="17">
         <f>C21*D21</f>
-        <v>86000</v>
+        <v>64000</v>
       </c>
       <c r="G21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="11" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="C22" s="17">
-        <v>20000</v>
+        <v>21500</v>
       </c>
       <c r="D22" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E22" s="17">
         <f>C22*D22</f>
-        <v>40000</v>
+        <v>86000</v>
       </c>
       <c r="G22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="9">
-        <f>SUM(E18:E22)</f>
+      <c r="B23" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="17">
+        <v>20000</v>
+      </c>
+      <c r="D23" s="3">
+        <v>2</v>
+      </c>
+      <c r="E23" s="17">
+        <f>C23*D23</f>
+        <v>40000</v>
+      </c>
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="9">
+        <f>SUM(E19:E23)</f>
         <v>416664</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B26" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C26" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D26" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E26" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="17">
-        <v>500</v>
-      </c>
-      <c r="D25" s="3">
-        <v>4</v>
-      </c>
-      <c r="E25" s="17">
-        <f>500</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="17">
-        <v>500</v>
-      </c>
-      <c r="D26" s="3">
-        <v>4</v>
-      </c>
-      <c r="E26" s="17">
-        <f>C26</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="11" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C27" s="17">
         <v>500</v>
@@ -1183,57 +1168,95 @@
         <v>4</v>
       </c>
       <c r="E27" s="17">
-        <f>C27</f>
+        <f>500</f>
         <v>500</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="9">
-        <f>SUM(E25:E27)</f>
+      <c r="B28" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="17">
+        <v>500</v>
+      </c>
+      <c r="D28" s="3">
+        <v>4</v>
+      </c>
+      <c r="E28" s="17">
+        <f>C28</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="17">
+        <v>500</v>
+      </c>
+      <c r="D29" s="3">
+        <v>4</v>
+      </c>
+      <c r="E29" s="17">
+        <f>C29</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="9">
+        <f>SUM(E27:E29)</f>
         <v>1500</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="9">
-        <f>SUM(E10,E23,E28)*0.03</f>
+      <c r="B32" s="9">
+        <f>SUM(E10,E24,E30)*0.03</f>
         <v>18200.941200000001</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="9">
-        <f>SUM(E10,E23,E28,B29)</f>
+      <c r="B33" s="9">
+        <f>SUM(E10,E24,E30,B32)</f>
         <v>624898.98120000004</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="22" t="s">
+    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="8">
-        <f>B30+operational!B25</f>
+      <c r="B36" s="8">
+        <f>B33+operational!B30</f>
         <v>2830334.5466</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="20" t="s">
+    <row r="37" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="21">
-        <f>(B30+operational!B25+'+ 18 months'!B25)</f>
+      <c r="B37" s="21">
+        <f>(B33+operational!B30+'+ 18 months'!B30)</f>
         <v>4545633.7</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1241,28 +1264,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFA28"/>
+  <dimension ref="A1:XFA33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12:H13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16381" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16381" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:16381" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16381" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="14" t="s">
         <v>1</v>
@@ -1277,7 +1300,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:16381" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16381" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -17668,7 +17691,7 @@
       <c r="XEZ3" s="3"/>
       <c r="XFA3" s="6"/>
     </row>
-    <row r="4" spans="1:16381" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16381" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
@@ -17683,7 +17706,7 @@
         <v>32346.899999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:16381" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16381" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
@@ -17698,7 +17721,7 @@
         <v>46227.78</v>
       </c>
     </row>
-    <row r="6" spans="1:16381" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16381" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="5"/>
       <c r="D6" s="3"/>
@@ -17707,306 +17730,307 @@
         <v>240574.68</v>
       </c>
     </row>
-    <row r="7" spans="1:16381" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:16381" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:16381" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12" t="s">
+    <row r="9" spans="1:16381" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C9" s="17">
         <v>1250</v>
-      </c>
-      <c r="D8" s="12">
-        <v>18</v>
-      </c>
-      <c r="E8" s="17">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16381" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="17">
-        <v>2000</v>
       </c>
       <c r="D9" s="12">
         <v>18</v>
       </c>
       <c r="E9" s="17">
-        <f>C9*D9</f>
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16381" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="17">
+        <v>2000</v>
+      </c>
+      <c r="D10" s="12">
+        <v>18</v>
+      </c>
+      <c r="E10" s="17">
+        <f>C10*D10</f>
         <v>36000</v>
       </c>
     </row>
-    <row r="10" spans="1:16381" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="18">
-        <f>SUM(E8:E9)</f>
+    <row r="11" spans="1:16381" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="18">
+        <f>SUM(E9:E10)</f>
         <v>37250</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H11" s="6"/>
     </row>
-    <row r="11" spans="1:16381" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="13" spans="1:16381" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E13" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="29"/>
+      <c r="H13" s="29"/>
     </row>
-    <row r="12" spans="1:16381" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12" t="s">
+    <row r="14" spans="1:16381" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="17">
-        <f>B28*0.03</f>
+      <c r="C14" s="17">
+        <f>B33*0.03</f>
         <v>34389.380399999995</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D14" s="12">
         <v>18</v>
       </c>
-      <c r="E12" s="30">
-        <f>C12*D12</f>
+      <c r="E14" s="30">
+        <f>C14*D14</f>
         <v>619008.84719999996</v>
       </c>
-      <c r="G12" s="32" t="s">
+      <c r="G14" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="H12" s="32"/>
+      <c r="H14" s="32"/>
     </row>
-    <row r="13" spans="1:16381" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12" t="s">
+    <row r="15" spans="1:16381" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="17">
-        <f>B28*0.02</f>
+      <c r="C15" s="17">
+        <f>B33*0.02</f>
         <v>22926.2536</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D15" s="12">
         <v>18</v>
       </c>
-      <c r="E13" s="17">
-        <f>C13*D13</f>
+      <c r="E15" s="17">
+        <f>C15*D15</f>
         <v>412672.56479999999</v>
       </c>
-      <c r="G13" s="32" t="s">
+      <c r="G15" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="32"/>
+      <c r="H15" s="32"/>
     </row>
-    <row r="14" spans="1:16381" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="18">
-        <f>SUM(E12:E13)</f>
+    <row r="16" spans="1:16381" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="18">
+        <f>SUM(E14:E15)</f>
         <v>1031681.412</v>
       </c>
     </row>
-    <row r="15" spans="1:16381" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:16381" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="3" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C19" s="4">
         <v>26666</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D19" s="3">
         <v>18</v>
       </c>
-      <c r="E16" s="6">
-        <f>C16*D16</f>
+      <c r="E19" s="6">
+        <f>C19*D19</f>
         <v>479988</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="3" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C20" s="4">
         <v>21500</v>
-      </c>
-      <c r="D17" s="3">
-        <v>18</v>
-      </c>
-      <c r="E17" s="17">
-        <f>C17*D17</f>
-        <v>387000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="18">
-        <f>SUM(E16:E17)</f>
-        <v>866988</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="17">
-        <v>500</v>
       </c>
       <c r="D20" s="3">
         <v>18</v>
       </c>
       <c r="E20" s="17">
-        <f>C20</f>
+        <f>C20*D20</f>
+        <v>387000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="18">
+        <f>SUM(E19:E20)</f>
+        <v>866988</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="17">
+        <v>500</v>
+      </c>
+      <c r="D24" s="3">
+        <v>18</v>
+      </c>
+      <c r="E24" s="17">
+        <f>C24</f>
         <v>500</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="11" t="s">
+    <row r="25" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C25" s="17">
         <v>500</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D25" s="3">
         <v>18</v>
       </c>
-      <c r="E21" s="17">
-        <f>C21</f>
+      <c r="E25" s="17">
+        <f>C25</f>
         <v>500</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="11" t="s">
+    <row r="26" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C26" s="17">
         <v>500</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D26" s="3">
         <v>18</v>
       </c>
-      <c r="E22" s="17">
-        <f>C22</f>
+      <c r="E26" s="17">
+        <f>C26</f>
         <v>500</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="18">
-        <f>SUM(E20:E22)</f>
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="18">
+        <f>SUM(E24:E26)</f>
         <v>1500</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="9">
-        <f>SUM(E5,E18,E23)*0.03</f>
+      <c r="B29" s="9">
+        <f>SUM(E5,E21,E27)*0.03</f>
         <v>27441.473399999999</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="18">
-        <f>SUM(E6,E14,E10,E18,B24,E23)</f>
+      <c r="B30" s="18">
+        <f>SUM(E6,E16,E11,E21,B29,E27)</f>
         <v>2205435.5654000002</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="18">
-        <f>SUM(E6,E10,E18,E23)</f>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="18">
+        <f>SUM(E6,E11,E21,E27)</f>
         <v>1146312.68</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C33" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18015,28 +18039,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD28"/>
+  <dimension ref="A1:XFD33"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13:H13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>23</v>
+    <row r="1" spans="1:16384" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="14" t="s">
         <v>1</v>
@@ -18051,7 +18075,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -34445,7 +34469,7 @@
       <c r="XFC3" s="3"/>
       <c r="XFD3" s="6"/>
     </row>
-    <row r="4" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
@@ -34460,7 +34484,7 @@
         <v>32346.899999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
@@ -34475,7 +34499,7 @@
         <v>46227.78</v>
       </c>
     </row>
-    <row r="6" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="5"/>
       <c r="D6" s="3"/>
@@ -34484,302 +34508,303 @@
         <v>240574.68</v>
       </c>
     </row>
-    <row r="7" spans="1:16384" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:16384" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:16384" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12" t="s">
+    <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C9" s="17">
         <v>1250</v>
-      </c>
-      <c r="D8" s="12">
-        <v>18</v>
-      </c>
-      <c r="E8" s="17">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16384" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="17">
-        <v>2000</v>
       </c>
       <c r="D9" s="12">
         <v>18</v>
       </c>
       <c r="E9" s="17">
-        <f>C9*D9</f>
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="17">
+        <v>2000</v>
+      </c>
+      <c r="D10" s="12">
+        <v>18</v>
+      </c>
+      <c r="E10" s="17">
+        <f>C10*D10</f>
         <v>36000</v>
       </c>
     </row>
-    <row r="10" spans="1:16384" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="18">
-        <f>SUM(E8:E9)</f>
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="18">
+        <f>SUM(E9:E10)</f>
         <v>37250</v>
       </c>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="13" spans="1:16384" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E13" s="19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:16384" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12" t="s">
+    <row r="14" spans="1:16384" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C14" s="17">
         <v>10000</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D14" s="12">
         <v>18</v>
       </c>
-      <c r="E12" s="17">
-        <f>C12*D12</f>
+      <c r="E14" s="17">
+        <f>C14*D14</f>
         <v>180000</v>
       </c>
-      <c r="G12" s="32" t="s">
+      <c r="G14" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="H12" s="32"/>
+      <c r="H14" s="32"/>
     </row>
-    <row r="13" spans="1:16384" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12" t="s">
+    <row r="15" spans="1:16384" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C15" s="17">
         <v>20000</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D15" s="12">
         <v>18</v>
       </c>
-      <c r="E13" s="17">
-        <f>C13*D13</f>
+      <c r="E15" s="17">
+        <f>C15*D15</f>
         <v>360000</v>
       </c>
-      <c r="G13" s="32" t="s">
+      <c r="G15" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="32"/>
+      <c r="H15" s="32"/>
     </row>
-    <row r="14" spans="1:16384" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="18">
-        <f>SUM(E12:E13)</f>
+    <row r="16" spans="1:16384" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="18">
+        <f>SUM(E14:E15)</f>
         <v>540000</v>
       </c>
     </row>
-    <row r="15" spans="1:16384" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:16384" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="3" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C19" s="4">
         <v>26666</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D19" s="3">
         <v>18</v>
       </c>
-      <c r="E16" s="6">
-        <f>C16*D16</f>
+      <c r="E19" s="6">
+        <f>C19*D19</f>
         <v>479988</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="3" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C20" s="4">
         <v>21500</v>
-      </c>
-      <c r="D17" s="3">
-        <v>18</v>
-      </c>
-      <c r="E17" s="17">
-        <f>C17*D17</f>
-        <v>387000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="18">
-        <f>SUM(E16:E17)</f>
-        <v>866988</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="17">
-        <v>500</v>
       </c>
       <c r="D20" s="3">
         <v>18</v>
       </c>
       <c r="E20" s="17">
-        <f>C20*2</f>
+        <f>C20*D20</f>
+        <v>387000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="18">
+        <f>SUM(E19:E20)</f>
+        <v>866988</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="17">
+        <v>500</v>
+      </c>
+      <c r="D24" s="3">
+        <v>18</v>
+      </c>
+      <c r="E24" s="17">
+        <f>C24*2</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="11" t="s">
+    <row r="25" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C25" s="17">
         <v>500</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D25" s="3">
         <v>18</v>
       </c>
-      <c r="E21" s="17">
-        <f>C21*2</f>
+      <c r="E25" s="17">
+        <f>C25*2</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="11" t="s">
+    <row r="26" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C26" s="17">
         <v>500</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D26" s="3">
         <v>18</v>
       </c>
-      <c r="E22" s="17">
-        <f>C22*2</f>
+      <c r="E26" s="17">
+        <f>C26*2</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="18">
-        <f>SUM(E20:E22)</f>
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="18">
+        <f>SUM(E24:E26)</f>
         <v>3000</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="9">
-        <f>SUM(E5,E18,E23)*0.03</f>
+      <c r="B29" s="9">
+        <f>SUM(E5,E21,E27)*0.03</f>
         <v>27486.473399999999</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="18">
-        <f>SUM(E6,E14,E10,E18,B24,E23)</f>
+      <c r="B30" s="18">
+        <f>SUM(E6,E16,E11,E21,B29,E27)</f>
         <v>1715299.1534</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="18">
-        <f>SUM(E6,E10,E18,E23)</f>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="18">
+        <f>SUM(E6,E11,E21,E27)</f>
         <v>1147812.68</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C33" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -34790,18 +34815,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
@@ -34809,7 +34834,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -34823,7 +34848,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -34831,7 +34856,7 @@
         <v>675663</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -34839,7 +34864,7 @@
         <v>535238</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -34847,7 +34872,7 @@
         <v>229303</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -34855,7 +34880,7 @@
         <v>176057</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -34863,13 +34888,13 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="22">
         <f>SUM(B2:B6)*0.03</f>
         <v>92740.26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -34878,7 +34903,7 @@
         <v>9274026</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
@@ -34886,7 +34911,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>47</v>
       </c>
@@ -34894,7 +34919,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
@@ -34902,7 +34927,7 @@
         <v>2.35E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
minor change in business startup cost
</commit_message>
<xml_diff>
--- a/Documentation/Business Startup Cost .xlsx
+++ b/Documentation/Business Startup Cost .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8505" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="pre" sheetId="1" r:id="rId1"/>
@@ -452,14 +452,14 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -17823,10 +17823,10 @@
         <f>C14*D14</f>
         <v>619008.84719999996</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="H14" s="32"/>
+      <c r="H14" s="33"/>
     </row>
     <row r="15" spans="1:16381" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
@@ -17844,10 +17844,10 @@
         <f>C15*D15</f>
         <v>412672.56479999999</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="G15" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="H15" s="32"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="16" spans="1:16381" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
@@ -18019,12 +18019,12 @@
         <f>SUM(E6,E11,E21,E27)</f>
         <v>1146312.68</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -18041,7 +18041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -18056,7 +18056,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="31" t="s">
         <v>63</v>
       </c>
     </row>
@@ -34598,10 +34598,10 @@
         <f>C14*D14</f>
         <v>180000</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="H14" s="32"/>
+      <c r="H14" s="33"/>
     </row>
     <row r="15" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
@@ -34618,10 +34618,10 @@
         <f>C15*D15</f>
         <v>360000</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="G15" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="H15" s="32"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="16" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
@@ -34793,12 +34793,12 @@
         <f>SUM(E6,E11,E21,E27)</f>
         <v>1147812.68</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -34815,15 +34815,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>